<commit_message>
Updated tests with new assert_footings_audit_xlsx_equal.
</commit_message>
<xml_diff>
--- a/tests/core/data/expected-integers.xlsx
+++ b/tests/core/data/expected-integers.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="IntegerModel" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="step_1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="step_2" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="step_3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IntegerModel" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="step_3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="__footings__" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -348,7 +349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,7 +370,7 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>Argument</t>
+          <t>Parameter</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -422,27 +423,44 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Step</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Return Type</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>Step</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Return Type</t>
+          <t>int</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Run step_1.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -452,14 +470,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Run step_1.</t>
+          <t>Run step_2.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_3</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -468,23 +486,6 @@
         </is>
       </c>
       <c r="D12" t="inlineStr">
-        <is>
-          <t>Run step_2.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>step_3</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
         <is>
           <t>Run step_3.</t>
         </is>
@@ -501,7 +502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C20"/>
+  <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,118 +517,91 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>Name:</t>
+          <t>Docstring:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>step_1</t>
-        </is>
-      </c>
+          <t>Run step_1.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Signature:</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>step_1(a, add)</t>
+          <t>Parameters</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>----------</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Docstring:</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Run step_1.</t>
+          <t>a : int</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
-          <t>Parameters</t>
+          <t>add : int</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>----------</t>
+          <t xml:space="preserve">    Amount to add</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>a : int</t>
-        </is>
-      </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number</t>
+          <t>Returns</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>add : int</t>
+          <t>-------</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Amount to add</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" t="inlineStr"/>
+          <t>int</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Returns</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>-------</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="B20" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C15" t="n">
         <v>2</v>
       </c>
     </row>
@@ -642,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C20"/>
+  <dimension ref="B2:C15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -657,118 +631,91 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>Name:</t>
+          <t>Docstring:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>step_2</t>
-        </is>
-      </c>
+          <t>Run step_2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Signature:</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>step_2(b, subtract)</t>
+          <t>Parameters</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>----------</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Docstring:</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Run step_2.</t>
+          <t>b : int</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
-          <t>Parameters</t>
+          <t>subtract : int</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>----------</t>
+          <t xml:space="preserve">    Amount to subtract</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>b : int</t>
-        </is>
-      </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number</t>
+          <t>Returns</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>subtract : int</t>
+          <t>-------</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Amount to subtract</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="C14" t="inlineStr"/>
+          <t>int</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Returns</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>-------</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="C18" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="B20" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -783,7 +730,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C22"/>
+  <dimension ref="B2:C17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,132 +745,1721 @@
     <row r="2">
       <c r="B2" t="inlineStr">
         <is>
-          <t>Name:</t>
+          <t>Docstring:</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>step_3</t>
-        </is>
-      </c>
+          <t>Run step_3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Signature:</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>step_3(a, b, c)</t>
+          <t>Parameters</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>----------</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Docstring:</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Run step_3.</t>
+          <t>a : int</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number A</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
-          <t>Parameters</t>
+          <t>b : int</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>----------</t>
+          <t xml:space="preserve">    A number B</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t>a : int</t>
+          <t>c : int</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number A</t>
+          <t xml:space="preserve">    A number C</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>b : int</t>
-        </is>
-      </c>
+      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number B</t>
+          <t>Returns</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t>c : int</t>
+          <t>-------</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number C</t>
-        </is>
+          <t>int</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Output:</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>worksheet</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dtype</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>row_start</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>col_start</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>row_end</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>col_end</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>IntegerModel</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>IntegerModel</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>&lt;class 'pandas.core.frame.DataFrame'&gt;</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>IntegerModel</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>&lt;class 'pandas.core.frame.DataFrame'&gt;</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3</v>
+      </c>
+      <c r="F14" t="n">
+        <v>6</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" t="n">
+        <v>7</v>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" t="n">
+        <v>8</v>
+      </c>
+      <c r="G16" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Returns</t>
-        </is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>9</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>-------</t>
-        </is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>int</t>
-        </is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>11</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>11</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>12</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3</v>
+      </c>
+      <c r="F20" t="n">
+        <v>12</v>
+      </c>
+      <c r="G20" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>13</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3</v>
+      </c>
+      <c r="F21" t="n">
+        <v>13</v>
+      </c>
+      <c r="G21" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="22">
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Output:</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>15</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>15</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>15</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>15</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>&lt;class 'int'&gt;</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>15</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>15</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>2</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>5</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>6</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3</v>
+      </c>
+      <c r="F34" t="n">
+        <v>6</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>7</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3</v>
+      </c>
+      <c r="F35" t="n">
+        <v>7</v>
+      </c>
+      <c r="G35" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>8</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3</v>
+      </c>
+      <c r="F36" t="n">
+        <v>8</v>
+      </c>
+      <c r="G36" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>9</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3</v>
+      </c>
+      <c r="F37" t="n">
+        <v>9</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>10</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3</v>
+      </c>
+      <c r="F38" t="n">
+        <v>10</v>
+      </c>
+      <c r="G38" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>11</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3</v>
+      </c>
+      <c r="F39" t="n">
+        <v>11</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>12</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3</v>
+      </c>
+      <c r="F40" t="n">
+        <v>12</v>
+      </c>
+      <c r="G40" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>13</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" t="n">
+        <v>13</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>15</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3</v>
+      </c>
+      <c r="F42" t="n">
+        <v>15</v>
+      </c>
+      <c r="G42" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>15</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="n">
+        <v>15</v>
+      </c>
+      <c r="G43" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>&lt;class 'int'&gt;</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>15</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3</v>
+      </c>
+      <c r="F44" t="n">
+        <v>15</v>
+      </c>
+      <c r="G44" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" t="n">
+        <v>2</v>
+      </c>
+      <c r="G45" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>2</v>
+      </c>
+      <c r="G46" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>2</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2</v>
+      </c>
+      <c r="F47" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>2</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2</v>
+      </c>
+      <c r="F49" t="n">
+        <v>2</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>2</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3</v>
+      </c>
+      <c r="F50" t="n">
+        <v>2</v>
+      </c>
+      <c r="G50" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>3</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>4</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3</v>
+      </c>
+      <c r="F52" t="n">
+        <v>4</v>
+      </c>
+      <c r="G52" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>5</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3</v>
+      </c>
+      <c r="F53" t="n">
+        <v>5</v>
+      </c>
+      <c r="G53" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>6</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3</v>
+      </c>
+      <c r="F54" t="n">
+        <v>6</v>
+      </c>
+      <c r="G54" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>7</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3</v>
+      </c>
+      <c r="F55" t="n">
+        <v>7</v>
+      </c>
+      <c r="G55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>8</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3</v>
+      </c>
+      <c r="F56" t="n">
+        <v>8</v>
+      </c>
+      <c r="G56" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>9</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3</v>
+      </c>
+      <c r="F57" t="n">
+        <v>9</v>
+      </c>
+      <c r="G57" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>10</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3</v>
+      </c>
+      <c r="F58" t="n">
+        <v>10</v>
+      </c>
+      <c r="G58" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>11</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3</v>
+      </c>
+      <c r="F59" t="n">
+        <v>11</v>
+      </c>
+      <c r="G59" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>12</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" t="n">
+        <v>12</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>13</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3</v>
+      </c>
+      <c r="F61" t="n">
+        <v>13</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>14</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3</v>
+      </c>
+      <c r="F62" t="n">
+        <v>14</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>15</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3</v>
+      </c>
+      <c r="F63" t="n">
+        <v>15</v>
+      </c>
+      <c r="G63" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>17</v>
+      </c>
+      <c r="E64" t="n">
+        <v>3</v>
+      </c>
+      <c r="F64" t="n">
+        <v>17</v>
+      </c>
+      <c r="G64" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>17</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2</v>
+      </c>
+      <c r="F65" t="n">
+        <v>17</v>
+      </c>
+      <c r="G65" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>&lt;class 'int'&gt;</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>17</v>
+      </c>
+      <c r="E66" t="n">
+        <v>3</v>
+      </c>
+      <c r="F66" t="n">
+        <v>17</v>
+      </c>
+      <c r="G66" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improvements to the aesthetics of generating xlsx audit files.
</commit_message>
<xml_diff>
--- a/tests/core/data/expected-integers.xlsx
+++ b/tests/core/data/expected-integers.xlsx
@@ -21,13 +21,26 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <i val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,14 +60,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="bold" xfId="1" hidden="0"/>
+    <cellStyle name="underline" xfId="2" hidden="0"/>
+    <cellStyle name="hyperlink" xfId="3" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
@@ -349,7 +371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:C32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -358,140 +380,214 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="2.14" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Model Name:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>IntegerModel</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Parameter</t>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Signature:</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
+          <t>IntegerModel(*, a, b, c) -&gt; 'IntegerModel'</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Docstring:</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Parameters</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>description for a</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
+    </row>
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    description for a</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
         <is>
           <t>b</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>description for b</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    description for b</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>description for c</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Step</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Return Type</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    description for c</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>Steps</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="3" t="inlineStr">
         <is>
           <t>step_1</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Run step_1.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Run step_1.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>step_2</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Run step_2.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Run step_2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t>step_3</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>int</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Run step_3.</t>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Run step_3.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>Methods</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>run()</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Executes the model.</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="C27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Returns</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    int</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>audit(file, **kwargs)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Creates an audit xlsx or json file.</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C17" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C19" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C21" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -502,7 +598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,97 +607,118 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="2.14" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="1" customWidth="1" min="3" max="3"/>
+    <col width="1.2" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Step Name:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>step_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Signature:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>step_1(a, add)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>Docstring:</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Run step_1.</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="C4" t="inlineStr">
+    <row r="7">
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Parameters</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>----------</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>a : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>add : int</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Amount to add</t>
+          <t>a : int</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>Returns</t>
+          <t>add : int</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>-------</t>
+          <t xml:space="preserve">    Amount to add</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Returns</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
         <is>
           <t>int</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
+    <row r="16">
+      <c r="C16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="1" t="inlineStr">
         <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="D18" t="n">
         <v>2</v>
       </c>
     </row>
@@ -616,7 +733,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,97 +742,118 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="2.14" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="1" customWidth="1" min="3" max="3"/>
+    <col width="1.2" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Step Name:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Signature:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>step_2(b, subtract)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>Docstring:</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Run step_2.</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="C4" t="inlineStr">
+    <row r="7">
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Parameters</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>----------</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>b : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>subtract : int</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Amount to subtract</t>
+          <t>b : int</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>Returns</t>
+          <t>subtract : int</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>-------</t>
+          <t xml:space="preserve">    Amount to subtract</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="C13" t="inlineStr">
+      <c r="C13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Returns</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
         <is>
           <t>int</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
+    <row r="16">
+      <c r="C16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="1" t="inlineStr">
         <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="D18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -730,7 +868,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:C17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -739,111 +877,132 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="2.14" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="1" customWidth="1" min="3" max="3"/>
+    <col width="1.2" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
+    <row r="1"/>
     <row r="2">
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Step Name:</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3"/>
+    <row r="4">
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Signature:</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>step_3(a, b, c)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>Docstring:</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Run step_3.</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="C4" t="inlineStr">
+    <row r="7">
+      <c r="C7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>Parameters</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>----------</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>a : int</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    A number A</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>b : int</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number B</t>
+          <t>a : int</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="C10" t="inlineStr">
         <is>
-          <t>c : int</t>
+          <t xml:space="preserve">    A number A</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    A number C</t>
+          <t>b : int</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="C12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    A number B</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="C13" t="inlineStr">
         <is>
-          <t>Returns</t>
+          <t>c : int</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t>-------</t>
+          <t xml:space="preserve">    A number C</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="C15" t="inlineStr">
+      <c r="C15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>Returns</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
         <is>
           <t>int</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" t="inlineStr">
+    <row r="18">
+      <c r="C18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="1" t="inlineStr">
         <is>
           <t>Output:</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="D20" t="n">
         <v>3</v>
       </c>
     </row>
@@ -858,7 +1017,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,20 +1094,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>&lt;class 'pandas.core.frame.DataFrame'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -959,26 +1118,26 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>&lt;class 'pandas.core.frame.DataFrame'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -987,22 +1146,22 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1011,22 +1170,22 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1035,22 +1194,22 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1059,13 +1218,13 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G8" t="n">
         <v>3</v>
@@ -1074,7 +1233,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1083,22 +1242,22 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1107,13 +1266,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E10" t="n">
         <v>3</v>
       </c>
       <c r="F10" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="G10" t="n">
         <v>3</v>
@@ -1122,7 +1281,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1131,13 +1290,13 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
         <v>3</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G11" t="n">
         <v>3</v>
@@ -1146,7 +1305,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1155,13 +1314,13 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E12" t="n">
         <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G12" t="n">
         <v>3</v>
@@ -1170,7 +1329,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1179,13 +1338,13 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E13" t="n">
         <v>3</v>
       </c>
       <c r="F13" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G13" t="n">
         <v>3</v>
@@ -1194,7 +1353,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1203,13 +1362,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E14" t="n">
         <v>3</v>
       </c>
       <c r="F14" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G14" t="n">
         <v>3</v>
@@ -1218,7 +1377,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1227,13 +1386,13 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E15" t="n">
         <v>3</v>
       </c>
       <c r="F15" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G15" t="n">
         <v>3</v>
@@ -1242,7 +1401,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1251,13 +1410,13 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E16" t="n">
         <v>3</v>
       </c>
       <c r="F16" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G16" t="n">
         <v>3</v>
@@ -1266,7 +1425,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1275,13 +1434,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E17" t="n">
         <v>3</v>
       </c>
       <c r="F17" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G17" t="n">
         <v>3</v>
@@ -1290,7 +1449,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1299,13 +1458,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E18" t="n">
         <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G18" t="n">
         <v>3</v>
@@ -1314,7 +1473,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1323,13 +1482,13 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E19" t="n">
         <v>3</v>
       </c>
       <c r="F19" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G19" t="n">
         <v>3</v>
@@ -1338,7 +1497,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1347,13 +1506,13 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E20" t="n">
         <v>3</v>
       </c>
       <c r="F20" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G20" t="n">
         <v>3</v>
@@ -1362,7 +1521,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1371,13 +1530,13 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E21" t="n">
         <v>3</v>
       </c>
       <c r="F21" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G21" t="n">
         <v>3</v>
@@ -1386,7 +1545,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1395,13 +1554,13 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E22" t="n">
         <v>3</v>
       </c>
       <c r="F22" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G22" t="n">
         <v>3</v>
@@ -1410,7 +1569,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1419,37 +1578,37 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>step_1</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E24" t="n">
         <v>3</v>
       </c>
       <c r="F24" t="n">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G24" t="n">
         <v>3</v>
@@ -1458,7 +1617,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1467,22 +1626,22 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="G25" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1491,13 +1650,13 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E26" t="n">
         <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="G26" t="n">
         <v>3</v>
@@ -1506,7 +1665,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1515,22 +1674,22 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="G27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1539,13 +1698,13 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="E28" t="n">
         <v>3</v>
       </c>
       <c r="F28" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="G28" t="n">
         <v>3</v>
@@ -1554,7 +1713,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1563,22 +1722,22 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="G29" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1587,13 +1746,13 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E30" t="n">
         <v>3</v>
       </c>
       <c r="F30" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="G30" t="n">
         <v>3</v>
@@ -1602,7 +1761,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1611,13 +1770,13 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E31" t="n">
         <v>3</v>
       </c>
       <c r="F31" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="G31" t="n">
         <v>3</v>
@@ -1626,7 +1785,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1635,13 +1794,13 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="E32" t="n">
         <v>3</v>
       </c>
       <c r="F32" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="G32" t="n">
         <v>3</v>
@@ -1650,7 +1809,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>IntegerModel</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1659,13 +1818,13 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E33" t="n">
         <v>3</v>
       </c>
       <c r="F33" t="n">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="G33" t="n">
         <v>3</v>
@@ -1674,7 +1833,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1683,22 +1842,22 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1707,13 +1866,13 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E35" t="n">
         <v>3</v>
       </c>
       <c r="F35" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G35" t="n">
         <v>3</v>
@@ -1722,7 +1881,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1731,22 +1890,22 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G36" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1755,13 +1914,13 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E37" t="n">
         <v>3</v>
       </c>
       <c r="F37" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G37" t="n">
         <v>3</v>
@@ -1770,7 +1929,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1779,22 +1938,22 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F38" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1803,13 +1962,13 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E39" t="n">
         <v>3</v>
       </c>
       <c r="F39" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G39" t="n">
         <v>3</v>
@@ -1818,7 +1977,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1827,13 +1986,13 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E40" t="n">
         <v>3</v>
       </c>
       <c r="F40" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G40" t="n">
         <v>3</v>
@@ -1842,7 +2001,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1851,13 +2010,13 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E41" t="n">
         <v>3</v>
       </c>
       <c r="F41" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G41" t="n">
         <v>3</v>
@@ -1866,7 +2025,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1875,13 +2034,13 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E42" t="n">
         <v>3</v>
       </c>
       <c r="F42" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G42" t="n">
         <v>3</v>
@@ -1890,7 +2049,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1899,37 +2058,37 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>step_2</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>&lt;class 'int'&gt;</t>
+          <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E44" t="n">
         <v>3</v>
       </c>
       <c r="F44" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G44" t="n">
         <v>3</v>
@@ -1938,7 +2097,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1947,22 +2106,22 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1971,13 +2130,13 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E46" t="n">
         <v>3</v>
       </c>
       <c r="F46" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G46" t="n">
         <v>3</v>
@@ -1986,7 +2145,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1995,22 +2154,22 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F47" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G47" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2019,13 +2178,13 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E48" t="n">
         <v>3</v>
       </c>
       <c r="F48" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G48" t="n">
         <v>3</v>
@@ -2034,7 +2193,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2043,22 +2202,22 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F49" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="G49" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2067,13 +2226,13 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E50" t="n">
         <v>3</v>
       </c>
       <c r="F50" t="n">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="G50" t="n">
         <v>3</v>
@@ -2082,7 +2241,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2091,46 +2250,46 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F51" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="G51" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>&lt;class 'str'&gt;</t>
+          <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
       <c r="D52" t="n">
+        <v>18</v>
+      </c>
+      <c r="E52" t="n">
         <v>4</v>
       </c>
-      <c r="E52" t="n">
-        <v>3</v>
-      </c>
       <c r="F52" t="n">
+        <v>18</v>
+      </c>
+      <c r="G52" t="n">
         <v>4</v>
-      </c>
-      <c r="G52" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2139,22 +2298,22 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F53" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G53" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2163,13 +2322,13 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E54" t="n">
         <v>3</v>
       </c>
       <c r="F54" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G54" t="n">
         <v>3</v>
@@ -2178,7 +2337,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2187,22 +2346,22 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F55" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2211,13 +2370,13 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E56" t="n">
         <v>3</v>
       </c>
       <c r="F56" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G56" t="n">
         <v>3</v>
@@ -2226,7 +2385,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2235,22 +2394,22 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F57" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2259,13 +2418,13 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E58" t="n">
         <v>3</v>
       </c>
       <c r="F58" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G58" t="n">
         <v>3</v>
@@ -2274,7 +2433,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2283,13 +2442,13 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E59" t="n">
         <v>3</v>
       </c>
       <c r="F59" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G59" t="n">
         <v>3</v>
@@ -2298,7 +2457,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2307,13 +2466,13 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E60" t="n">
         <v>3</v>
       </c>
       <c r="F60" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G60" t="n">
         <v>3</v>
@@ -2322,7 +2481,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2331,13 +2490,13 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E61" t="n">
         <v>3</v>
       </c>
       <c r="F61" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G61" t="n">
         <v>3</v>
@@ -2346,7 +2505,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2355,13 +2514,13 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E62" t="n">
         <v>3</v>
       </c>
       <c r="F62" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G62" t="n">
         <v>3</v>
@@ -2370,7 +2529,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2379,13 +2538,13 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E63" t="n">
         <v>3</v>
       </c>
       <c r="F63" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G63" t="n">
         <v>3</v>
@@ -2394,7 +2553,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2403,13 +2562,13 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E64" t="n">
         <v>3</v>
       </c>
       <c r="F64" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G64" t="n">
         <v>3</v>
@@ -2418,7 +2577,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>step_3</t>
+          <t>step_2</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2427,40 +2586,664 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F65" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>14</v>
+      </c>
+      <c r="E66" t="n">
+        <v>3</v>
+      </c>
+      <c r="F66" t="n">
+        <v>14</v>
+      </c>
+      <c r="G66" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>15</v>
+      </c>
+      <c r="E67" t="n">
+        <v>3</v>
+      </c>
+      <c r="F67" t="n">
+        <v>15</v>
+      </c>
+      <c r="G67" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>16</v>
+      </c>
+      <c r="E68" t="n">
+        <v>3</v>
+      </c>
+      <c r="F68" t="n">
+        <v>16</v>
+      </c>
+      <c r="G68" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>17</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3</v>
+      </c>
+      <c r="F69" t="n">
+        <v>17</v>
+      </c>
+      <c r="G69" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>18</v>
+      </c>
+      <c r="E70" t="n">
+        <v>2</v>
+      </c>
+      <c r="F70" t="n">
+        <v>18</v>
+      </c>
+      <c r="G70" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>step_2</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>&lt;class 'int'&gt;</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>18</v>
+      </c>
+      <c r="E71" t="n">
+        <v>4</v>
+      </c>
+      <c r="F71" t="n">
+        <v>18</v>
+      </c>
+      <c r="G71" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
           <t>step_3</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>2</v>
+      </c>
+      <c r="E72" t="n">
+        <v>2</v>
+      </c>
+      <c r="F72" t="n">
+        <v>2</v>
+      </c>
+      <c r="G72" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>2</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G73" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>4</v>
+      </c>
+      <c r="E74" t="n">
+        <v>2</v>
+      </c>
+      <c r="F74" t="n">
+        <v>4</v>
+      </c>
+      <c r="G74" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>4</v>
+      </c>
+      <c r="E75" t="n">
+        <v>3</v>
+      </c>
+      <c r="F75" t="n">
+        <v>4</v>
+      </c>
+      <c r="G75" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>6</v>
+      </c>
+      <c r="E76" t="n">
+        <v>2</v>
+      </c>
+      <c r="F76" t="n">
+        <v>6</v>
+      </c>
+      <c r="G76" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>6</v>
+      </c>
+      <c r="E77" t="n">
+        <v>3</v>
+      </c>
+      <c r="F77" t="n">
+        <v>6</v>
+      </c>
+      <c r="G77" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>7</v>
+      </c>
+      <c r="E78" t="n">
+        <v>3</v>
+      </c>
+      <c r="F78" t="n">
+        <v>7</v>
+      </c>
+      <c r="G78" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>8</v>
+      </c>
+      <c r="E79" t="n">
+        <v>3</v>
+      </c>
+      <c r="F79" t="n">
+        <v>8</v>
+      </c>
+      <c r="G79" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>9</v>
+      </c>
+      <c r="E80" t="n">
+        <v>3</v>
+      </c>
+      <c r="F80" t="n">
+        <v>9</v>
+      </c>
+      <c r="G80" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>10</v>
+      </c>
+      <c r="E81" t="n">
+        <v>3</v>
+      </c>
+      <c r="F81" t="n">
+        <v>10</v>
+      </c>
+      <c r="G81" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>11</v>
+      </c>
+      <c r="E82" t="n">
+        <v>3</v>
+      </c>
+      <c r="F82" t="n">
+        <v>11</v>
+      </c>
+      <c r="G82" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>12</v>
+      </c>
+      <c r="E83" t="n">
+        <v>3</v>
+      </c>
+      <c r="F83" t="n">
+        <v>12</v>
+      </c>
+      <c r="G83" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>13</v>
+      </c>
+      <c r="E84" t="n">
+        <v>3</v>
+      </c>
+      <c r="F84" t="n">
+        <v>13</v>
+      </c>
+      <c r="G84" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>14</v>
+      </c>
+      <c r="E85" t="n">
+        <v>3</v>
+      </c>
+      <c r="F85" t="n">
+        <v>14</v>
+      </c>
+      <c r="G85" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>15</v>
+      </c>
+      <c r="E86" t="n">
+        <v>3</v>
+      </c>
+      <c r="F86" t="n">
+        <v>15</v>
+      </c>
+      <c r="G86" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>16</v>
+      </c>
+      <c r="E87" t="n">
+        <v>3</v>
+      </c>
+      <c r="F87" t="n">
+        <v>16</v>
+      </c>
+      <c r="G87" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>17</v>
+      </c>
+      <c r="E88" t="n">
+        <v>3</v>
+      </c>
+      <c r="F88" t="n">
+        <v>17</v>
+      </c>
+      <c r="G88" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>18</v>
+      </c>
+      <c r="E89" t="n">
+        <v>3</v>
+      </c>
+      <c r="F89" t="n">
+        <v>18</v>
+      </c>
+      <c r="G89" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>19</v>
+      </c>
+      <c r="E90" t="n">
+        <v>3</v>
+      </c>
+      <c r="F90" t="n">
+        <v>19</v>
+      </c>
+      <c r="G90" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>&lt;class 'str'&gt;</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>20</v>
+      </c>
+      <c r="E91" t="n">
+        <v>2</v>
+      </c>
+      <c r="F91" t="n">
+        <v>20</v>
+      </c>
+      <c r="G91" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>step_3</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
         <is>
           <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
-      <c r="D66" t="n">
-        <v>17</v>
-      </c>
-      <c r="E66" t="n">
-        <v>3</v>
-      </c>
-      <c r="F66" t="n">
-        <v>17</v>
-      </c>
-      <c r="G66" t="n">
-        <v>3</v>
+      <c r="D92" t="n">
+        <v>20</v>
+      </c>
+      <c r="E92" t="n">
+        <v>4</v>
+      </c>
+      <c r="F92" t="n">
+        <v>20</v>
+      </c>
+      <c r="G92" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added __footings_attribute_map__ as attribute under model to be used.
</commit_message>
<xml_diff>
--- a/tests/core/data/expected-integers.xlsx
+++ b/tests/core/data/expected-integers.xlsx
@@ -739,7 +739,7 @@
   <cols>
     <col width="2.14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="24" customWidth="1" min="3" max="3"/>
+    <col width="29" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -791,7 +791,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[a, b]</t>
+          <t>[parameter.a, parameter.b]</t>
         </is>
       </c>
     </row>
@@ -804,7 +804,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[ret_1]</t>
+          <t>[asset.ret_1]</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ret_1</t>
+          <t>asset.ret_1</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -858,7 +858,7 @@
   <cols>
     <col width="2.14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="29" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
@@ -910,7 +910,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[c, d]</t>
+          <t>[parameter.c, parameter.d]</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[ret_2]</t>
+          <t>[asset.ret_2]</t>
         </is>
       </c>
     </row>
@@ -949,7 +949,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ret_2</t>
+          <t>asset.ret_2</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[ret_1, ret_2]</t>
+          <t>[asset.ret_1, asset.ret_2]</t>
         </is>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[ret_3]</t>
+          <t>[asset.ret_3]</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ret_3</t>
+          <t>asset.ret_3</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -2900,7 +2900,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>[ret_1]</t>
+          <t>[asset.ret_1]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>[ret_1]</t>
+          <t>[asset.ret_1]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -3355,7 +3355,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[ret_2]</t>
+          <t>[asset.ret_2]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3394,7 +3394,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[ret_2]</t>
+          <t>[asset.ret_2]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -3810,7 +3810,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>[ret_3]</t>
+          <t>[asset.ret_3]</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3849,7 +3849,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>[ret_3]</t>
+          <t>[asset.ret_3]</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">

</xml_diff>